<commit_message>
Se actualiza diagrama de Gantt
</commit_message>
<xml_diff>
--- a/Auto/A- Material Aulico/Diagrama de Gantt del proyecto A.C.R.I.Co.xlsx
+++ b/Auto/A- Material Aulico/Diagrama de Gantt del proyecto A.C.R.I.Co.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F3A7DD-490B-4D90-A9F5-894CB34FE2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9FA9D9-EED8-4E03-A072-64EC128A34B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento de proyecto" sheetId="4" r:id="rId1"/>
@@ -30,12 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Cree un seguimiento de proyecto en esta hoja de cálculo.
 El título de esta hoja de cálculo se encuentra en la celda B1. 
@@ -62,10 +59,6 @@
 La siguiente instrucción se encuentra en la celda A22.</t>
   </si>
   <si>
-    <t>Para agregar más hitos o actividades, inserte filas nuevas encima de esta línea.
-Esta es la última instrucción de esta hoja de cálculo.</t>
-  </si>
-  <si>
     <t>Seguimiento de proyecto</t>
   </si>
   <si>
@@ -170,6 +163,12 @@
   </si>
   <si>
     <t>Presentacion de proyecto y división de tareas</t>
+  </si>
+  <si>
+    <t>Se puso en funcionamiento el sensor MQ2</t>
+  </si>
+  <si>
+    <t>Ensayo y prueba de funcionamiento</t>
   </si>
 </sst>
 </file>
@@ -182,7 +181,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +324,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,12 +348,6 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -713,7 +718,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0">
@@ -734,42 +739,42 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -777,7 +782,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -798,7 +803,6 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -809,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="4">
@@ -817,6 +821,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="4" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30" customBuiltin="1"/>
@@ -870,41 +880,12 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -933,14 +914,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1053,6 +1026,43 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1281,7 +1291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C77E71CD-5CF6-486A-B4E9-E4D50FBD7182}" type="CELLRANGE">
+                    <a:fld id="{19645D23-49F5-4A63-B525-759C4BEE8F48}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1315,7 +1325,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:r>
-                      <a:rPr lang="es-AR"/>
+                      <a:rPr lang="en-US"/>
                       <a:t>Presentación de proyecto y división de tareas</a:t>
                     </a:r>
                   </a:p>
@@ -1343,7 +1353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{590FEFE0-AB4B-4E45-8B26-B70FDBE18CAB}" type="CELLRANGE">
+                    <a:fld id="{45581C28-1F82-4E75-B787-E3C6C101389A}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1376,7 +1386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{585DC6AC-2F7E-4F73-AF3D-494A5B3F899A}" type="CELLRANGE">
+                    <a:fld id="{F53BFFC5-6936-4EB3-98B9-62EDA1CD626C}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1409,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB7AC573-CF6A-42D5-8E56-F2FA6C3CA5ED}" type="CELLRANGE">
+                    <a:fld id="{60695871-3C95-4D44-BD50-C14AB7008CC4}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2309,13 +2319,13 @@
       <xdr:twoCellAnchor editAs="absolute">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:colOff>175260</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
-          <xdr:colOff>438150</xdr:colOff>
+          <xdr:colOff>441960</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -2358,23 +2368,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Hitos" displayName="Hitos" ref="B4:G20">
-  <autoFilter ref="B4:G20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G21">
-    <sortCondition ref="C6:C21"/>
-    <sortCondition ref="D6:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Hitos" displayName="Hitos" ref="B4:G16">
+  <autoFilter ref="B4:G16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G17">
+    <sortCondition ref="C6:C17"/>
+    <sortCondition ref="D6:D17"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Posición" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha de inicio" totalsRowDxfId="10" dataCellStyle="Date"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fecha de finalización" totalsRowDxfId="9" dataCellStyle="Date"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Posición" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha de inicio" totalsRowDxfId="5" dataCellStyle="Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fecha de finalización" totalsRowDxfId="4" dataCellStyle="Date"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Hito o actividad">
       <calculatedColumnFormula>"Actividad"&amp;" "&amp;ROW($A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Inicio el día" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Inicio el día" dataDxfId="2" totalsRowDxfId="3">
       <calculatedColumnFormula>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C5)-INT($C$5)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Duración de la tarea" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Duración de la tarea" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1">
       <calculatedColumnFormula>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2388,7 +2398,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DatosDinámicos" displayName="DatosDinámicos" ref="B5:E10" totalsRowShown="0" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DatosDinámicos" displayName="DatosDinámicos" ref="B5:E10" totalsRowShown="0" tableBorderDxfId="12">
   <autoFilter ref="B5:E10" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2396,16 +2406,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="hito" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="hito" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,4)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="fecha" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="fecha" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$C5,$B$3,0,1,1))=0,End_Date,INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Inicio el día" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Inicio el día" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$F5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,5)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="duración" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="duración" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$G5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,6)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2684,52 +2694,52 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
     <col min="5" max="5" width="52" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="15">
         <v>44809</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="15">
         <f ca="1">IFERROR(IF(MAX(Hitos[Fecha de finalización])=0,TODAY(),MAX(Hitos[Fecha de finalización])),TODAY())</f>
@@ -2737,355 +2747,296 @@
       </c>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>44809</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>44809</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="23">
+        <v>26</v>
+      </c>
+      <c r="F5" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C5)-INT($C$5)),"")</f>
         <v>0</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>44810</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>44810</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="23">
+        <v>36</v>
+      </c>
+      <c r="F6" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C6)-INT($C$5)),"")</f>
         <v>1</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>44811</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>44813</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="23">
+        <v>32</v>
+      </c>
+      <c r="F7" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C7)-INT($C$5)),"")</f>
         <v>2</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>44814</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>44815</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="23">
+        <v>28</v>
+      </c>
+      <c r="F8" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C8)-INT($C$5)),"")</f>
         <v>5</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="21">
         <v>5</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>44816</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>44816</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="23">
+        <v>29</v>
+      </c>
+      <c r="F9" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C9)-INT($C$5)),"")</f>
         <v>7</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="21">
         <v>6</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>44817</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>44817</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="23">
+        <v>30</v>
+      </c>
+      <c r="F10" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C10)-INT($C$5)),"")</f>
         <v>8</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
         <v>7</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>44818</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>44821</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="23">
+        <v>35</v>
+      </c>
+      <c r="F11" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C11)-INT($C$5)),"")</f>
         <v>9</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="21">
         <v>8</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>44822</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <v>44822</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="23">
+        <v>31</v>
+      </c>
+      <c r="F12" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C12)-INT($C$5)),"")</f>
         <v>13</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="26">
         <v>9</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="27">
         <v>44823</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="27">
         <v>44824</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="23">
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C13)-INT($C$5)),"")</f>
         <v>14</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="21">
         <v>10</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>44825</v>
       </c>
-      <c r="D14" s="24">
-        <v>44827</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="D14" s="23">
+        <v>44825</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C14)-INT($C$5)),"")</f>
         <v>16</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="21">
         <v>11</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="23" t="str">
+      <c r="C15" s="23">
+        <v>44826</v>
+      </c>
+      <c r="D15" s="23">
+        <v>44826</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C15)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G15" s="23" t="str">
+        <v>17</v>
+      </c>
+      <c r="G15" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="22">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="21">
         <v>12</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="23" t="str">
+      <c r="C16" s="23">
+        <v>44827</v>
+      </c>
+      <c r="D16" s="23">
+        <v>44827</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="22">
         <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C16)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G16" s="23" t="str">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22">
         <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
-        <v>13</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="23" t="str">
-        <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C17)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="23" t="str">
-        <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
-        <v>14</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="23" t="str">
-        <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C18)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G18" s="23" t="str">
-        <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
-        <v>15</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="23" t="str">
-        <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C19)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G19" s="23" t="str">
-        <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="23" t="str">
-        <f>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C20)-INT($C$5)),"")</f>
-        <v/>
-      </c>
-      <c r="G20" s="23" t="str">
-        <f>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3105,22 +3056,22 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>14</v>
+    <row r="1" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3140,13 +3091,13 @@
                 <anchor>
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:colOff>175260</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>13</xdr:col>
-                    <xdr:colOff>438150</xdr:colOff>
+                    <xdr:colOff>441960</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </to>
@@ -3170,68 +3121,68 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,4)),"")</f>
         <v>Debate, selección de problemática y su posible solución</v>
@@ -3249,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E6,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B6+$B$3,4)),"")</f>
         <v>Presentacion de proyecto y división de tareas</v>
@@ -3267,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E7,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B7+$B$3,4)),"")</f>
         <v>Compra de materiales</v>
@@ -3285,8 +3236,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
       <c r="B9" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E8,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B8+$B$3,4)),"")</f>
         <v>Construcción del chasis del auto</v>
@@ -3304,8 +3255,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
       <c r="B10" s="13" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E9,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B9+$B$3,4)),"")</f>
         <v>Instalación de las ruedas, los motores y puente H al chasis</v>

</xml_diff>

<commit_message>
Se agregan diagramas de Gantt
</commit_message>
<xml_diff>
--- a/Auto/A- Material Aulico/Diagrama de Gantt del proyecto A.C.R.I.Co.xlsx
+++ b/Auto/A- Material Aulico/Diagrama de Gantt del proyecto A.C.R.I.Co.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9FA9D9-EED8-4E03-A072-64EC128A34B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E08F9-CCB1-4D3A-B0D1-0BE770F7075B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,12 +880,41 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -914,6 +943,14 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1026,43 +1063,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1291,7 +1291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19645D23-49F5-4A63-B525-759C4BEE8F48}" type="CELLRANGE">
+                    <a:fld id="{8418FF20-08FE-4BB8-AF0C-FA2656DDB481}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1353,7 +1353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45581C28-1F82-4E75-B787-E3C6C101389A}" type="CELLRANGE">
+                    <a:fld id="{805F8650-F23A-4890-A89A-9D72FDD7E914}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1386,7 +1386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F53BFFC5-6936-4EB3-98B9-62EDA1CD626C}" type="CELLRANGE">
+                    <a:fld id="{70F3691B-DAD8-4762-82FC-5D13FDF9199E}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1419,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60695871-3C95-4D44-BD50-C14AB7008CC4}" type="CELLRANGE">
+                    <a:fld id="{E300A3A5-40CF-4DF1-A2EF-1CFE325F7F1A}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2375,16 +2375,16 @@
     <sortCondition ref="D6:D17"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Posición" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha de inicio" totalsRowDxfId="5" dataCellStyle="Date"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fecha de finalización" totalsRowDxfId="4" dataCellStyle="Date"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Posición" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha de inicio" totalsRowDxfId="10" dataCellStyle="Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fecha de finalización" totalsRowDxfId="9" dataCellStyle="Date"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Hito o actividad">
       <calculatedColumnFormula>"Actividad"&amp;" "&amp;ROW($A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Inicio el día" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Inicio el día" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IFERROR(IF(OR(LEN(Hitos[[#This Row],[Fecha de inicio]])=0,LEN(Hitos[[#This Row],[Fecha de finalización]])=0),"",INT(C5)-INT($C$5)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Duración de la tarea" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Duración de la tarea" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>IFERROR(IF(Hitos[[#This Row],[Inicio el día]]=0,DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1,IF(LEN(Hitos[[#This Row],[Inicio el día]])=0,"",DATEDIF(Hitos[[#This Row],[Fecha de inicio]],Hitos[[#This Row],[Fecha de finalización]],"d")+1)),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2398,7 +2398,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DatosDinámicos" displayName="DatosDinámicos" ref="B5:E10" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DatosDinámicos" displayName="DatosDinámicos" ref="B5:E10" totalsRowShown="0" tableBorderDxfId="4">
   <autoFilter ref="B5:E10" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2406,16 +2406,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="hito" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="hito" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$E5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,4)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="fecha" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="fecha" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$C5,$B$3,0,1,1))=0,End_Date,INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Inicio el día" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Inicio el día" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$F5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,5)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="duración" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="duración" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Seguimiento de proyecto'!$G5,$B$3,0,1,1))=0,"",INDEX(Hitos[],'Seguimiento de proyecto'!$B5+$B$3,6)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>

</xml_diff>